<commit_message>
started Qi unittests; added Zi parse quat tests
</commit_message>
<xml_diff>
--- a/misc/progress_tracker.xlsx
+++ b/misc/progress_tracker.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredreich/Documents/Projects/github/gaussian_integers/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredreich/Documents/Projects/github/gaussian_integers/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEE23ED-B5EE-1447-9826-017384E88C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC02D0F-1EDA-904C-8428-B5AF9C81194E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="680" windowWidth="20900" windowHeight="16980" xr2:uid="{CD64052E-6ECC-8E41-B63D-E5B1F34E7651}"/>
+    <workbookView xWindow="5320" yWindow="600" windowWidth="22140" windowHeight="16980" xr2:uid="{CD64052E-6ECC-8E41-B63D-E5B1F34E7651}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="92">
   <si>
     <t>__abs__</t>
   </si>
@@ -405,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -425,13 +426,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -440,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -461,9 +459,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -501,7 +499,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -607,7 +605,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -749,7 +747,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -763,12 +761,12 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.83203125" style="1" customWidth="1"/>
@@ -790,7 +788,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <f ca="1">NOW()</f>
-        <v>45949.603016203706</v>
+        <v>45951.534407870371</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>57</v>
@@ -820,12 +818,12 @@
       <c r="D3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G3" s="7"/>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>87</v>
       </c>
     </row>
@@ -838,7 +836,7 @@
       <c r="D4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
         <v>59</v>
       </c>
@@ -846,7 +844,7 @@
       <c r="H4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>89</v>
       </c>
     </row>
@@ -856,10 +854,10 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
         <v>59</v>
       </c>
@@ -867,7 +865,7 @@
       <c r="H5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="10" t="s">
         <v>88</v>
       </c>
     </row>
@@ -880,15 +878,17 @@
       <c r="D6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F6" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>90</v>
       </c>
     </row>
@@ -896,19 +896,19 @@
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="9"/>
+      <c r="B7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="8" t="s">
         <v>86</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="13"/>
+      <c r="H7" s="12"/>
       <c r="I7" t="s">
         <v>91</v>
       </c>
@@ -917,12 +917,12 @@
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
         <v>59</v>
       </c>
@@ -932,12 +932,12 @@
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="9"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
@@ -945,14 +945,14 @@
       <c r="A10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="9"/>
+      <c r="B10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="8" t="s">
         <v>86</v>
       </c>
@@ -962,14 +962,14 @@
       <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="9"/>
+      <c r="B11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="8" t="s">
         <v>86</v>
       </c>
@@ -979,12 +979,12 @@
       <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
@@ -992,12 +992,12 @@
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
@@ -1005,31 +1005,33 @@
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="9"/>
+      <c r="B14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>59</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="12" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
         <v>59</v>
       </c>
@@ -1039,12 +1041,12 @@
       <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
@@ -1052,14 +1054,14 @@
       <c r="A17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="9"/>
+      <c r="B17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E17" s="9"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="8" t="s">
         <v>86</v>
       </c>
@@ -1069,14 +1071,14 @@
       <c r="A18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="9"/>
+      <c r="B18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="7"/>
       <c r="D18" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="8" t="s">
         <v>86</v>
       </c>
@@ -1086,10 +1088,10 @@
       <c r="A19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="9"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
@@ -1097,12 +1099,12 @@
       <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
         <v>59</v>
       </c>
@@ -1112,14 +1114,14 @@
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="9"/>
+      <c r="B21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="9"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="8" t="s">
         <v>86</v>
       </c>
@@ -1129,12 +1131,14 @@
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="9"/>
+      <c r="E22" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F22" s="7" t="s">
         <v>59</v>
       </c>
@@ -1144,12 +1148,12 @@
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="9"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
         <v>59</v>
       </c>
@@ -1159,12 +1163,12 @@
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="9"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="7" t="s">
         <v>59</v>
       </c>
@@ -1174,12 +1178,12 @@
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="9"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
         <v>59</v>
       </c>
@@ -1189,14 +1193,14 @@
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="9"/>
+      <c r="B26" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="7"/>
       <c r="D26" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E26" s="9"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="8" t="s">
         <v>86</v>
       </c>
@@ -1206,12 +1210,12 @@
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="9"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
@@ -1219,12 +1223,12 @@
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="9"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
         <v>59</v>
       </c>
@@ -1234,12 +1238,12 @@
       <c r="A29" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="9"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="7" t="s">
         <v>59</v>
       </c>
@@ -1249,12 +1253,12 @@
       <c r="A30" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="9"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="7" t="s">
         <v>59</v>
       </c>
@@ -1264,12 +1268,12 @@
       <c r="A31" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
       <c r="D31" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="9"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="7" t="s">
         <v>59</v>
       </c>
@@ -1279,10 +1283,10 @@
       <c r="A32" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="9"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="7" t="s">
         <v>59</v>
       </c>
@@ -1292,12 +1296,12 @@
       <c r="A33" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33" s="9"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
     </row>
@@ -1305,12 +1309,14 @@
       <c r="A34" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
       <c r="D34" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="9"/>
+      <c r="E34" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
     </row>
@@ -1318,12 +1324,12 @@
       <c r="A35" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="9"/>
+      <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
         <v>59</v>
       </c>
@@ -1333,10 +1339,10 @@
       <c r="A36" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="9"/>
+      <c r="E36" s="7"/>
       <c r="F36" s="7" t="s">
         <v>59</v>
       </c>
@@ -1346,12 +1352,12 @@
       <c r="A37" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="9"/>
+      <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
@@ -1359,12 +1365,12 @@
       <c r="A38" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="9"/>
+      <c r="E38" s="7"/>
       <c r="F38" s="7" t="s">
         <v>59</v>
       </c>
@@ -1374,10 +1380,10 @@
       <c r="A39" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="9"/>
+      <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
     </row>
@@ -1385,31 +1391,35 @@
       <c r="A40" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="9"/>
+      <c r="B40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="7"/>
       <c r="D40" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="9"/>
+      <c r="E40" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F40" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G40" s="7"/>
+      <c r="G40" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="9"/>
+      <c r="B41" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="7"/>
       <c r="D41" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="9"/>
+      <c r="E41" s="7"/>
       <c r="F41" s="8" t="s">
         <v>86</v>
       </c>
@@ -1419,12 +1429,12 @@
       <c r="A42" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="9"/>
+      <c r="E42" s="7"/>
       <c r="F42" s="7" t="s">
         <v>59</v>
       </c>
@@ -1434,12 +1444,12 @@
       <c r="A43" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="9"/>
+      <c r="E43" s="7"/>
       <c r="F43" s="7" t="s">
         <v>59</v>
       </c>
@@ -1449,14 +1459,14 @@
       <c r="A44" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="9"/>
+      <c r="B44" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="7"/>
       <c r="D44" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="9"/>
+      <c r="E44" s="7"/>
       <c r="F44" s="8" t="s">
         <v>86</v>
       </c>
@@ -1466,10 +1476,10 @@
       <c r="A45" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="9"/>
+      <c r="E45" s="7"/>
       <c r="F45" s="7" t="s">
         <v>59</v>
       </c>
@@ -1479,10 +1489,10 @@
       <c r="A46" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="9"/>
+      <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
     </row>
@@ -1490,12 +1500,14 @@
       <c r="A47" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
       <c r="D47" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E47" s="9"/>
+      <c r="E47" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F47" s="7" t="s">
         <v>59</v>
       </c>
@@ -1505,14 +1517,16 @@
       <c r="A48" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="9"/>
+      <c r="B48" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="7"/>
       <c r="D48" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="9"/>
+      <c r="E48" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F48" s="8" t="s">
         <v>86</v>
       </c>
@@ -1522,12 +1536,12 @@
       <c r="A49" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="12" t="s">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E49" s="9"/>
+      <c r="E49" s="7"/>
       <c r="F49" s="7" t="s">
         <v>59</v>
       </c>
@@ -1537,10 +1551,10 @@
       <c r="A50" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="9"/>
+      <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
     </row>
@@ -1548,14 +1562,16 @@
       <c r="A51" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="9"/>
+      <c r="B51" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="7"/>
       <c r="D51" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="9"/>
+      <c r="E51" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F51" s="8" t="s">
         <v>86</v>
       </c>
@@ -1565,10 +1581,10 @@
       <c r="A52" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="7"/>
-      <c r="E52" s="9"/>
+      <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
@@ -1576,14 +1592,16 @@
       <c r="A53" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" s="9"/>
+      <c r="B53" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="7"/>
       <c r="D53" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E53" s="9"/>
+      <c r="E53" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F53" s="8" t="s">
         <v>86</v>
       </c>
@@ -1593,14 +1611,16 @@
       <c r="A54" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="9"/>
+      <c r="B54" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="7"/>
       <c r="D54" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E54" s="9"/>
+      <c r="E54" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F54" s="8" t="s">
         <v>86</v>
       </c>
@@ -1610,14 +1630,14 @@
       <c r="A55" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="9"/>
+      <c r="B55" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="7"/>
       <c r="D55" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E55" s="9"/>
+      <c r="E55" s="7"/>
       <c r="F55" s="8" t="s">
         <v>86</v>
       </c>
@@ -1627,10 +1647,10 @@
       <c r="A56" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
       <c r="D56" s="7"/>
-      <c r="E56" s="9"/>
+      <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
     </row>
@@ -1638,12 +1658,12 @@
       <c r="A57" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
       <c r="D57" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E57" s="9"/>
+      <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
     </row>
@@ -1651,12 +1671,12 @@
       <c r="A58" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="12" t="s">
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E58" s="9"/>
+      <c r="E58" s="7"/>
       <c r="F58" s="7" t="s">
         <v>59</v>
       </c>
@@ -1666,10 +1686,10 @@
       <c r="A59" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
       <c r="D59" s="7"/>
-      <c r="E59" s="9"/>
+      <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
     </row>
@@ -1677,14 +1697,16 @@
       <c r="A60" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="9"/>
+      <c r="B60" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="7"/>
       <c r="D60" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E60" s="9"/>
+      <c r="E60" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F60" s="8" t="s">
         <v>86</v>
       </c>
@@ -1694,10 +1716,10 @@
       <c r="A61" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
       <c r="D61" s="7"/>
-      <c r="E61" s="9"/>
+      <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
     </row>
@@ -1705,12 +1727,12 @@
       <c r="A62" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
       <c r="D62" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E62" s="9"/>
+      <c r="E62" s="7"/>
       <c r="F62" s="7" t="s">
         <v>59</v>
       </c>
@@ -1720,14 +1742,16 @@
       <c r="A63" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C63" s="9"/>
+      <c r="B63" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="7"/>
       <c r="D63" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E63" s="9"/>
+      <c r="E63" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F63" s="8" t="s">
         <v>86</v>
       </c>
@@ -1737,12 +1761,14 @@
       <c r="A64" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
       <c r="D64" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E64" s="9"/>
+      <c r="E64" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
     </row>
@@ -1750,12 +1776,12 @@
       <c r="A65" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
       <c r="D65" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E65" s="9"/>
+      <c r="E65" s="7"/>
       <c r="F65" s="7" t="s">
         <v>59</v>
       </c>
@@ -1765,12 +1791,12 @@
       <c r="A66" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
       <c r="D66" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E66" s="9"/>
+      <c r="E66" s="7"/>
       <c r="F66" s="7" t="s">
         <v>59</v>
       </c>
@@ -1780,12 +1806,14 @@
       <c r="A67" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
       <c r="D67" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E67" s="9"/>
+      <c r="E67" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F67" s="7" t="s">
         <v>59</v>
       </c>
@@ -1795,12 +1823,12 @@
       <c r="A68" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
       <c r="D68" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E68" s="9"/>
+      <c r="E68" s="7"/>
       <c r="F68" s="7" t="s">
         <v>59</v>
       </c>
@@ -1810,12 +1838,12 @@
       <c r="A69" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
       <c r="D69" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E69" s="9"/>
+      <c r="E69" s="7"/>
       <c r="F69" s="7" t="s">
         <v>59</v>
       </c>
@@ -1825,14 +1853,16 @@
       <c r="A70" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B70" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C70" s="9"/>
+      <c r="B70" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" s="7"/>
       <c r="D70" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E70" s="9"/>
+      <c r="E70" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F70" s="8" t="s">
         <v>86</v>
       </c>
@@ -1842,14 +1872,16 @@
       <c r="A71" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B71" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C71" s="9"/>
+      <c r="B71" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="7"/>
       <c r="D71" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E71" s="9"/>
+      <c r="E71" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F71" s="8" t="s">
         <v>86</v>
       </c>
@@ -1859,12 +1891,12 @@
       <c r="A72" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="12" t="s">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E72" s="9"/>
+      <c r="E72" s="7"/>
       <c r="F72" s="7" t="s">
         <v>59</v>
       </c>
@@ -1874,10 +1906,10 @@
       <c r="A73" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
       <c r="D73" s="7"/>
-      <c r="E73" s="9"/>
+      <c r="E73" s="7"/>
       <c r="F73" s="7" t="s">
         <v>59</v>
       </c>
@@ -1887,14 +1919,16 @@
       <c r="A74" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B74" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C74" s="9"/>
+      <c r="B74" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C74" s="7"/>
       <c r="D74" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E74" s="9"/>
+      <c r="E74" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F74" s="8" t="s">
         <v>86</v>
       </c>
@@ -1904,10 +1938,10 @@
       <c r="A75" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
       <c r="D75" s="7"/>
-      <c r="E75" s="9"/>
+      <c r="E75" s="7"/>
       <c r="F75" s="7" t="s">
         <v>59</v>
       </c>
@@ -1917,12 +1951,14 @@
       <c r="A76" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
       <c r="D76" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E76" s="9"/>
+      <c r="E76" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
@@ -1930,12 +1966,12 @@
       <c r="A77" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E77" s="9"/>
+      <c r="E77" s="7"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
     </row>
@@ -1943,10 +1979,10 @@
       <c r="A78" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
       <c r="D78" s="7"/>
-      <c r="E78" s="9"/>
+      <c r="E78" s="7"/>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
     </row>
@@ -1954,12 +1990,14 @@
       <c r="A79" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
       <c r="D79" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E79" s="9"/>
+      <c r="E79" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="F79" s="7" t="s">
         <v>59</v>
       </c>
@@ -1969,12 +2007,12 @@
       <c r="A80" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E80" s="9"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
     </row>

</xml_diff>